<commit_message>
update on a draft graph
- tabs for main page (graph), methods, dataset table
- texts on main page
- dataset table draft (in progress table)
- filters on graph
- dataset preparation: cleaning, short project names, exclusion of projects older than 2020, sdg (?)
</commit_message>
<xml_diff>
--- a/data/cs_edges.xlsx
+++ b/data/cs_edges.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="107">
   <si>
     <t>from</t>
   </si>
@@ -111,19 +111,259 @@
   </si>
   <si>
     <t>s22</t>
+  </si>
+  <si>
+    <t>s23</t>
+  </si>
+  <si>
+    <t>s24</t>
+  </si>
+  <si>
+    <t>s25</t>
+  </si>
+  <si>
+    <t>s26</t>
+  </si>
+  <si>
+    <t>s27</t>
+  </si>
+  <si>
+    <t>s28</t>
+  </si>
+  <si>
+    <t>s29</t>
+  </si>
+  <si>
+    <t>s30</t>
+  </si>
+  <si>
+    <t>s31</t>
+  </si>
+  <si>
+    <t>s32</t>
+  </si>
+  <si>
+    <t>s33</t>
+  </si>
+  <si>
+    <t>s34</t>
+  </si>
+  <si>
+    <t>s35</t>
+  </si>
+  <si>
+    <t>s36</t>
+  </si>
+  <si>
+    <t>s37</t>
+  </si>
+  <si>
+    <t>s38</t>
+  </si>
+  <si>
+    <t>s39</t>
+  </si>
+  <si>
+    <t>s40</t>
+  </si>
+  <si>
+    <t>s41</t>
+  </si>
+  <si>
+    <t>s42</t>
+  </si>
+  <si>
+    <t>s43</t>
+  </si>
+  <si>
+    <t>s44</t>
+  </si>
+  <si>
+    <t>s45</t>
+  </si>
+  <si>
+    <t>s46</t>
+  </si>
+  <si>
+    <t>s47</t>
+  </si>
+  <si>
+    <t>project_short</t>
+  </si>
+  <si>
+    <t>Technische Universität Berlin</t>
+  </si>
+  <si>
+    <t>Freie Universität Berlin</t>
+  </si>
+  <si>
+    <t>Humboldt-Universität zu Berlin</t>
+  </si>
+  <si>
+    <t>Charité – Universitätsmedizin Berlin</t>
+  </si>
+  <si>
+    <t>Mind the Fungi!</t>
+  </si>
+  <si>
+    <t>Deine emotionale Stadt</t>
+  </si>
+  <si>
+    <t>Blühender Campus FU</t>
+  </si>
+  <si>
+    <t>Citizen Science @FESSTVaL</t>
+  </si>
+  <si>
+    <t>SimRa: Sicherheit im Radverkehr</t>
+  </si>
+  <si>
+    <t>Freemove</t>
+  </si>
+  <si>
+    <t>Humboldt Explorers</t>
+  </si>
+  <si>
+    <t>Open Heritage</t>
+  </si>
+  <si>
+    <t>NutriGreen</t>
+  </si>
+  <si>
+    <t>RECIPES</t>
+  </si>
+  <si>
+    <t>Ginkoo</t>
+  </si>
+  <si>
+    <t>EDiCitNet</t>
+  </si>
+  <si>
+    <t>Open Urban Climate Observatory Berlin</t>
+  </si>
+  <si>
+    <t>StadtUmMig</t>
+  </si>
+  <si>
+    <t>Stadtarboretum</t>
+  </si>
+  <si>
+    <t>Urbane Klima-Gärten</t>
+  </si>
+  <si>
+    <t>Stadtlabor for Multimodal Anthropology</t>
+  </si>
+  <si>
+    <t>Polytopia</t>
+  </si>
+  <si>
+    <t>Schmeck-Projekt</t>
+  </si>
+  <si>
+    <t>BerlinAir NO2-Atlas</t>
+  </si>
+  <si>
+    <t>Virtual LimitLab</t>
+  </si>
+  <si>
+    <t>SlcGA</t>
+  </si>
+  <si>
+    <t>co2libri</t>
+  </si>
+  <si>
+    <t>DOPMADE</t>
+  </si>
+  <si>
+    <t>Trash Games</t>
+  </si>
+  <si>
+    <t>Urban Citizenship-Making at Times of Crisis</t>
+  </si>
+  <si>
+    <t>De:link // Re:link</t>
+  </si>
+  <si>
+    <t>KEEP COOL</t>
+  </si>
+  <si>
+    <t>TRAIN 4 Science</t>
+  </si>
+  <si>
+    <t>Theater des Anthropozän</t>
+  </si>
+  <si>
+    <t>Die Wildenbruch-Werkstatt</t>
+  </si>
+  <si>
+    <t>PerSociety</t>
+  </si>
+  <si>
+    <t>Berlin Spricht!</t>
+  </si>
+  <si>
+    <t>STÄLECODIA</t>
+  </si>
+  <si>
+    <t>Städtisches Leben Während Corona</t>
+  </si>
+  <si>
+    <t>Transforming with Fungi</t>
+  </si>
+  <si>
+    <t>MY-CO BUILD+AFFECT</t>
+  </si>
+  <si>
+    <t>MY-CO PLACE</t>
+  </si>
+  <si>
+    <t>Reste der Reste</t>
+  </si>
+  <si>
+    <t>MY-CO SPACE</t>
+  </si>
+  <si>
+    <t>B-Part</t>
+  </si>
+  <si>
+    <t>Patient:innen-zentrierte Forshcung der Ergebnissekommunikation</t>
+  </si>
+  <si>
+    <t>„Happy in Berlin? English Writers in the City, The 1920s and Beyond.“</t>
+  </si>
+  <si>
+    <t>Design Thinking in der Lehrkräftebildung</t>
+  </si>
+  <si>
+    <t>Water4Whom</t>
+  </si>
+  <si>
+    <t>SAGRaS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boddenhecht </t>
+  </si>
+  <si>
+    <t>uni</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,7 +374,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -142,15 +382,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC1C7D0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFC1C7D0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFC1C7D0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -431,319 +691,975 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="33.61328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.84375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1">
+      <c r="E4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1">
+      <c r="E6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1">
+      <c r="E7" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="1">
+      <c r="E11" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="1">
+      <c r="E12" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="1">
+      <c r="E23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="1">
+      <c r="E24" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="1">
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>